<commit_message>
fix several headers that weren't named in right format
</commit_message>
<xml_diff>
--- a/MI_Barry/MI_Barry_GE20_cleaned.xlsx
+++ b/MI_Barry/MI_Barry_GE20_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Barry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B997793-7C2C-44B8-B238-70ADB78EE662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C51CAFA-572F-437F-94DB-77F5F4E5394C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="300" windowWidth="33690" windowHeight="18760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19390" yWindow="1370" windowWidth="15910" windowHeight="18760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="51">
-  <si>
-    <t>Precinct</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="49">
   <si>
     <t>City of Hastings, Precinct 1H</t>
   </si>
@@ -102,82 +99,79 @@
     <t>Yankee Springs Township, Precinct 2</t>
   </si>
   <si>
+    <t>precinct</t>
+  </si>
+  <si>
+    <t>Democratic Party - DEM</t>
+  </si>
+  <si>
+    <t>Republican Party - REP</t>
+  </si>
+  <si>
+    <t>Libertarian Party - LIB</t>
+  </si>
+  <si>
+    <t>U.S. Taxpayers Party - UST</t>
+  </si>
+  <si>
+    <t>Working Class Party - WCP</t>
+  </si>
+  <si>
+    <t>Green Party - GRN</t>
+  </si>
+  <si>
+    <t>Natural Law Party - NLP</t>
+  </si>
+  <si>
+    <t>WriteIn</t>
+  </si>
+  <si>
+    <t>Joseph R. Biden - DEM</t>
+  </si>
+  <si>
+    <t>Donald J. Trump - REP</t>
+  </si>
+  <si>
+    <t>Jo Jorgensen - LIB</t>
+  </si>
+  <si>
+    <t>Don Blankenship - UST</t>
+  </si>
+  <si>
+    <t>Howie Hawkins - GRN</t>
+  </si>
+  <si>
+    <t>Rocky De La Fuente - NAT</t>
+  </si>
+  <si>
+    <t>Gary Peters - DEM</t>
+  </si>
+  <si>
+    <t>John James - REP</t>
+  </si>
+  <si>
+    <t>Valerie L. Willis - UST</t>
+  </si>
+  <si>
+    <t>Marcia Squier - GRN</t>
+  </si>
+  <si>
+    <t>Doug Dern - NAT</t>
+  </si>
+  <si>
+    <t>Hillary Scholten - DEM</t>
+  </si>
+  <si>
+    <t>Peter Meijer - REP</t>
+  </si>
+  <si>
+    <t>Jay Molette - DEM</t>
+  </si>
+  <si>
+    <t>Julie A. Calley - REP</t>
+  </si>
+  <si>
     <t>Ballots Cast</t>
-  </si>
-  <si>
-    <t>Registered Voters</t>
-  </si>
-  <si>
-    <t>precinct</t>
-  </si>
-  <si>
-    <t>Democratic Party - DEM</t>
-  </si>
-  <si>
-    <t>Republican Party - REP</t>
-  </si>
-  <si>
-    <t>Libertarian Party - LIB</t>
-  </si>
-  <si>
-    <t>U.S. Taxpayers Party - UST</t>
-  </si>
-  <si>
-    <t>Working Class Party - WCP</t>
-  </si>
-  <si>
-    <t>Green Party - GRN</t>
-  </si>
-  <si>
-    <t>Natural Law Party - NLP</t>
-  </si>
-  <si>
-    <t>WriteIn</t>
-  </si>
-  <si>
-    <t>Joseph R. Biden - DEM</t>
-  </si>
-  <si>
-    <t>Donald J. Trump - REP</t>
-  </si>
-  <si>
-    <t>Jo Jorgensen - LIB</t>
-  </si>
-  <si>
-    <t>Don Blankenship - UST</t>
-  </si>
-  <si>
-    <t>Howie Hawkins - GRN</t>
-  </si>
-  <si>
-    <t>Rocky De La Fuente - NAT</t>
-  </si>
-  <si>
-    <t>Gary Peters - DEM</t>
-  </si>
-  <si>
-    <t>John James - REP</t>
-  </si>
-  <si>
-    <t>Valerie L. Willis - UST</t>
-  </si>
-  <si>
-    <t>Marcia Squier - GRN</t>
-  </si>
-  <si>
-    <t>Doug Dern - NAT</t>
-  </si>
-  <si>
-    <t>Hillary Scholten - DEM</t>
-  </si>
-  <si>
-    <t>Peter Meijer - REP</t>
-  </si>
-  <si>
-    <t>Jay Molette - DEM</t>
-  </si>
-  <si>
-    <t>Julie A. Calley - REP</t>
   </si>
 </sst>
 </file>
@@ -557,291 +551,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0708A30-01EA-44C8-B78F-CC9E58A94384}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
         <v>1061</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
         <v>840</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
         <v>856</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
         <v>1051</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>2032</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
       <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
         <v>1458</v>
       </c>
     </row>
@@ -855,7 +773,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -873,36 +791,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>195</v>
@@ -931,7 +849,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>130</v>
@@ -960,7 +878,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>121</v>
@@ -989,7 +907,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>192</v>
@@ -1018,7 +936,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>148</v>
@@ -1047,7 +965,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>126</v>
@@ -1076,7 +994,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>280</v>
@@ -1105,7 +1023,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>207</v>
@@ -1134,7 +1052,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>230</v>
@@ -1163,7 +1081,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>234</v>
@@ -1192,7 +1110,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>266</v>
@@ -1221,7 +1139,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>241</v>
@@ -1250,7 +1168,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>294</v>
@@ -1279,7 +1197,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>96</v>
@@ -1308,7 +1226,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>352</v>
@@ -1337,7 +1255,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>376</v>
@@ -1366,7 +1284,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>173</v>
@@ -1395,7 +1313,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>263</v>
@@ -1424,7 +1342,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>203</v>
@@ -1453,7 +1371,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>148</v>
@@ -1482,7 +1400,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>349</v>
@@ -1511,7 +1429,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>190</v>
@@ -1540,7 +1458,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>259</v>
@@ -1569,7 +1487,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>210</v>
@@ -1606,7 +1524,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1622,33 +1540,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>480</v>
@@ -1674,7 +1592,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>318</v>
@@ -1700,7 +1618,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>335</v>
@@ -1726,7 +1644,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>473</v>
@@ -1752,7 +1670,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>274</v>
@@ -1778,7 +1696,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>283</v>
@@ -1804,7 +1722,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>700</v>
@@ -1830,7 +1748,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>425</v>
@@ -1856,7 +1774,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>457</v>
@@ -1882,7 +1800,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>555</v>
@@ -1908,7 +1826,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>621</v>
@@ -1934,7 +1852,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>583</v>
@@ -1960,7 +1878,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>578</v>
@@ -1986,7 +1904,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>191</v>
@@ -2012,7 +1930,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>645</v>
@@ -2038,7 +1956,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>817</v>
@@ -2064,7 +1982,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>378</v>
@@ -2090,7 +2008,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>581</v>
@@ -2116,7 +2034,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>549</v>
@@ -2142,7 +2060,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>357</v>
@@ -2168,7 +2086,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>757</v>
@@ -2194,7 +2112,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>409</v>
@@ -2220,7 +2138,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>567</v>
@@ -2246,7 +2164,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>464</v>
@@ -2296,30 +2214,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>442</v>
@@ -2342,7 +2260,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>310</v>
@@ -2365,7 +2283,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>313</v>
@@ -2388,7 +2306,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>456</v>
@@ -2411,7 +2329,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>284</v>
@@ -2434,7 +2352,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>279</v>
@@ -2457,7 +2375,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>649</v>
@@ -2480,7 +2398,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>414</v>
@@ -2503,7 +2421,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>473</v>
@@ -2526,7 +2444,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>557</v>
@@ -2549,7 +2467,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>619</v>
@@ -2572,7 +2490,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>571</v>
@@ -2595,7 +2513,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>579</v>
@@ -2618,7 +2536,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>183</v>
@@ -2641,7 +2559,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>625</v>
@@ -2664,7 +2582,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>771</v>
@@ -2687,7 +2605,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>367</v>
@@ -2710,7 +2628,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>540</v>
@@ -2733,7 +2651,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>497</v>
@@ -2756,7 +2674,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>341</v>
@@ -2779,7 +2697,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>722</v>
@@ -2802,7 +2720,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>408</v>
@@ -2825,7 +2743,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>535</v>
@@ -2848,7 +2766,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>434</v>
@@ -2891,21 +2809,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>472</v>
@@ -2919,7 +2837,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>329</v>
@@ -2933,7 +2851,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>349</v>
@@ -2947,7 +2865,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>468</v>
@@ -2961,7 +2879,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>289</v>
@@ -2975,7 +2893,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>330</v>
@@ -2989,7 +2907,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>701</v>
@@ -3003,7 +2921,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>441</v>
@@ -3017,7 +2935,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>471</v>
@@ -3031,7 +2949,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>579</v>
@@ -3045,7 +2963,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>663</v>
@@ -3059,7 +2977,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>614</v>
@@ -3073,7 +2991,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>613</v>
@@ -3087,7 +3005,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>205</v>
@@ -3101,7 +3019,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>669</v>
@@ -3115,7 +3033,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>804</v>
@@ -3129,7 +3047,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>378</v>
@@ -3143,7 +3061,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>574</v>
@@ -3157,7 +3075,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>543</v>
@@ -3171,7 +3089,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>352</v>
@@ -3185,7 +3103,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>788</v>
@@ -3199,7 +3117,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>394</v>
@@ -3213,7 +3131,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>587</v>
@@ -3227,7 +3145,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>445</v>
@@ -3249,7 +3167,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3261,21 +3179,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>366</v>
@@ -3289,7 +3207,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>266</v>
@@ -3303,7 +3221,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>279</v>
@@ -3317,7 +3235,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>381</v>
@@ -3331,7 +3249,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>234</v>
@@ -3345,7 +3263,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>225</v>
@@ -3359,7 +3277,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>568</v>
@@ -3373,7 +3291,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>332</v>
@@ -3387,7 +3305,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>390</v>
@@ -3401,7 +3319,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>457</v>
@@ -3415,7 +3333,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>518</v>
@@ -3429,7 +3347,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>479</v>
@@ -3443,7 +3361,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>501</v>
@@ -3457,7 +3375,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>154</v>
@@ -3471,7 +3389,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>558</v>
@@ -3485,7 +3403,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>692</v>
@@ -3499,7 +3417,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>303</v>
@@ -3513,7 +3431,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>453</v>
@@ -3527,7 +3445,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>444</v>
@@ -3541,7 +3459,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>289</v>
@@ -3555,7 +3473,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>654</v>
@@ -3569,7 +3487,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>311</v>
@@ -3583,7 +3501,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>486</v>
@@ -3597,7 +3515,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>392</v>

</xml_diff>